<commit_message>
Support for x,y-insensitive off-sheet references.
</commit_message>
<xml_diff>
--- a/ExceLintTests/TestData/AddressModes.xlsx
+++ b/ExceLintTests/TestData/AddressModes.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>input</t>
   </si>
@@ -36,6 +37,9 @@
   </si>
   <si>
     <t>broken</t>
+  </si>
+  <si>
+    <t>off-sheet single</t>
   </si>
 </sst>
 </file>
@@ -387,15 +391,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -408,8 +412,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -425,8 +432,12 @@
         <f>SUM($A$2:A5)</f>
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <f>Sheet2!$A$2</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -442,8 +453,12 @@
         <f>SUM(A$2:A5)</f>
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <f>Sheet2!A$2</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -459,8 +474,12 @@
         <f>SUM($A2:A5)</f>
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <f>Sheet2!$A2</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -471,6 +490,45 @@
       <c r="C5">
         <f>SUM(A2:A5)</f>
         <v>10</v>
+      </c>
+      <c r="E5">
+        <f>Sheet2!A2</f>
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>